<commit_message>
adding small acl analysis
</commit_message>
<xml_diff>
--- a/data/raw/collected_metadata/metadata_avis.xlsx
+++ b/data/raw/collected_metadata/metadata_avis.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="1524" documentId="11_AD4D9D64A577C15A4A54185C681B52125BDEDD8A" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BEEAB86F-1843-49A5-8F07-AF9A8FBF02E8}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-90" yWindow="0" windowWidth="11380" windowHeight="13370" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="metadata" sheetId="1" r:id="rId1"/>
@@ -2013,25 +2013,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P146"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A106" zoomScale="75" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="O103" sqref="O103"/>
+    <sheetView tabSelected="1" topLeftCell="A38" zoomScale="75" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="K61" sqref="K61"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="14.42578125" customWidth="1"/>
-    <col min="3" max="3" width="20.140625" customWidth="1"/>
-    <col min="4" max="4" width="11.7109375" customWidth="1"/>
-    <col min="5" max="5" width="13.42578125" customWidth="1"/>
-    <col min="6" max="6" width="16.7109375" customWidth="1"/>
-    <col min="7" max="7" width="7.5703125" customWidth="1"/>
+    <col min="2" max="2" width="14.453125" customWidth="1"/>
+    <col min="3" max="3" width="20.1796875" customWidth="1"/>
+    <col min="4" max="4" width="11.7265625" customWidth="1"/>
+    <col min="5" max="5" width="13.453125" customWidth="1"/>
+    <col min="6" max="6" width="16.7265625" customWidth="1"/>
+    <col min="7" max="7" width="7.54296875" customWidth="1"/>
     <col min="8" max="8" width="9" customWidth="1"/>
-    <col min="9" max="9" width="11.85546875" customWidth="1"/>
-    <col min="10" max="10" width="30.42578125" customWidth="1"/>
-    <col min="11" max="11" width="17.28515625" customWidth="1"/>
+    <col min="9" max="9" width="11.81640625" customWidth="1"/>
+    <col min="10" max="10" width="30.453125" customWidth="1"/>
+    <col min="11" max="11" width="17.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2081,7 +2081,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>144</v>
       </c>
@@ -2132,7 +2132,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>143</v>
       </c>
@@ -2180,7 +2180,7 @@
         <v>547</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>142</v>
       </c>
@@ -2227,7 +2227,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>141</v>
       </c>
@@ -2274,7 +2274,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>140</v>
       </c>
@@ -2315,7 +2315,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>139</v>
       </c>
@@ -2362,7 +2362,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>138</v>
       </c>
@@ -2403,7 +2403,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>137</v>
       </c>
@@ -2444,7 +2444,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>136</v>
       </c>
@@ -2485,7 +2485,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>135</v>
       </c>
@@ -2532,7 +2532,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>134</v>
       </c>
@@ -2576,7 +2576,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>133</v>
       </c>
@@ -2617,7 +2617,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>132</v>
       </c>
@@ -2664,7 +2664,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>131</v>
       </c>
@@ -2711,7 +2711,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>130</v>
       </c>
@@ -2758,7 +2758,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>129</v>
       </c>
@@ -2802,7 +2802,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>128</v>
       </c>
@@ -2846,7 +2846,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>127</v>
       </c>
@@ -2887,7 +2887,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>126</v>
       </c>
@@ -2928,7 +2928,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>125</v>
       </c>
@@ -2969,7 +2969,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>124</v>
       </c>
@@ -3010,7 +3010,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>123</v>
       </c>
@@ -3057,7 +3057,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>122</v>
       </c>
@@ -3101,7 +3101,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>121</v>
       </c>
@@ -3151,7 +3151,7 @@
         <v>548</v>
       </c>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>120</v>
       </c>
@@ -3195,7 +3195,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>119</v>
       </c>
@@ -3242,7 +3242,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>118</v>
       </c>
@@ -3289,7 +3289,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>117</v>
       </c>
@@ -3333,7 +3333,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>116</v>
       </c>
@@ -3374,7 +3374,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>115</v>
       </c>
@@ -3415,7 +3415,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A32">
         <v>114</v>
       </c>
@@ -3462,7 +3462,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A33">
         <v>113</v>
       </c>
@@ -3503,7 +3503,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A34">
         <v>112</v>
       </c>
@@ -3547,7 +3547,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A35">
         <v>111</v>
       </c>
@@ -3594,7 +3594,7 @@
         <v>537</v>
       </c>
     </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A36">
         <v>110</v>
       </c>
@@ -3638,7 +3638,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A37">
         <v>109</v>
       </c>
@@ -3682,7 +3682,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A38">
         <v>108</v>
       </c>
@@ -3729,7 +3729,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A39">
         <v>107</v>
       </c>
@@ -3770,7 +3770,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A40">
         <v>106</v>
       </c>
@@ -3817,7 +3817,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A41">
         <v>105</v>
       </c>
@@ -3861,7 +3861,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A42">
         <v>104</v>
       </c>
@@ -3908,7 +3908,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="43" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A43">
         <v>103</v>
       </c>
@@ -3958,7 +3958,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="44" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A44">
         <v>102</v>
       </c>
@@ -4008,7 +4008,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="45" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A45">
         <v>101</v>
       </c>
@@ -4049,7 +4049,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A46">
         <v>100</v>
       </c>
@@ -4099,7 +4099,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="47" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A47">
         <v>99</v>
       </c>
@@ -4146,7 +4146,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="48" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A48">
         <v>98</v>
       </c>
@@ -4190,7 +4190,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A49">
         <v>97</v>
       </c>
@@ -4240,7 +4240,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="50" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A50">
         <v>96</v>
       </c>
@@ -4284,7 +4284,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A51">
         <v>95</v>
       </c>
@@ -4334,7 +4334,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="52" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A52">
         <v>94</v>
       </c>
@@ -4384,7 +4384,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="53" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A53">
         <v>93</v>
       </c>
@@ -4431,7 +4431,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="54" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A54">
         <v>92</v>
       </c>
@@ -4481,7 +4481,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="55" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A55">
         <v>91</v>
       </c>
@@ -4531,7 +4531,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="56" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A56">
         <v>90</v>
       </c>
@@ -4575,7 +4575,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A57">
         <v>89</v>
       </c>
@@ -4622,7 +4622,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A58">
         <v>88</v>
       </c>
@@ -4672,7 +4672,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="59" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A59">
         <v>87</v>
       </c>
@@ -4713,7 +4713,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A60">
         <v>86</v>
       </c>
@@ -4760,7 +4760,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A61">
         <v>85</v>
       </c>
@@ -4807,7 +4807,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A62">
         <v>84</v>
       </c>
@@ -4857,7 +4857,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="63" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A63">
         <v>83</v>
       </c>
@@ -4907,7 +4907,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="64" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A64">
         <v>82</v>
       </c>
@@ -4957,7 +4957,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="65" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A65">
         <v>81</v>
       </c>
@@ -5004,7 +5004,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A66">
         <v>80</v>
       </c>
@@ -5054,7 +5054,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="67" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A67">
         <v>79</v>
       </c>
@@ -5101,7 +5101,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A68">
         <v>78</v>
       </c>
@@ -5151,7 +5151,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="69" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A69">
         <v>77</v>
       </c>
@@ -5195,7 +5195,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="70" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A70">
         <v>76</v>
       </c>
@@ -5242,7 +5242,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A71">
         <v>75</v>
       </c>
@@ -5289,7 +5289,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="72" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A72">
         <v>74</v>
       </c>
@@ -5339,7 +5339,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="73" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A73">
         <v>73</v>
       </c>
@@ -5389,7 +5389,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="74" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A74">
         <v>72</v>
       </c>
@@ -5436,7 +5436,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="75" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A75">
         <v>71</v>
       </c>
@@ -5486,7 +5486,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="76" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A76">
         <v>70</v>
       </c>
@@ -5527,7 +5527,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A77">
         <v>69</v>
       </c>
@@ -5568,7 +5568,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A78">
         <v>68</v>
       </c>
@@ -5618,7 +5618,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="79" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A79">
         <v>67</v>
       </c>
@@ -5665,7 +5665,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="80" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A80">
         <v>66</v>
       </c>
@@ -5715,7 +5715,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="81" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A81">
         <v>65</v>
       </c>
@@ -5762,7 +5762,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="82" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A82">
         <v>64</v>
       </c>
@@ -5812,7 +5812,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="83" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A83">
         <v>63</v>
       </c>
@@ -5856,7 +5856,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="84" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A84">
         <v>62</v>
       </c>
@@ -5906,7 +5906,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="85" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A85">
         <v>61</v>
       </c>
@@ -5947,7 +5947,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A86">
         <v>60</v>
       </c>
@@ -5991,7 +5991,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A87">
         <v>59</v>
       </c>
@@ -6032,7 +6032,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="88" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A88">
         <v>58</v>
       </c>
@@ -6076,7 +6076,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A89">
         <v>57</v>
       </c>
@@ -6117,7 +6117,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="90" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A90">
         <v>56</v>
       </c>
@@ -6158,7 +6158,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A91">
         <v>55</v>
       </c>
@@ -6202,7 +6202,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A92">
         <v>54</v>
       </c>
@@ -6246,7 +6246,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A93">
         <v>53</v>
       </c>
@@ -6287,7 +6287,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A94">
         <v>52</v>
       </c>
@@ -6328,7 +6328,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A95">
         <v>51</v>
       </c>
@@ -6372,7 +6372,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="96" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A96">
         <v>50</v>
       </c>
@@ -6416,7 +6416,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A97">
         <v>49</v>
       </c>
@@ -6460,7 +6460,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A98">
         <v>48</v>
       </c>
@@ -6507,7 +6507,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="99" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A99">
         <v>47</v>
       </c>
@@ -6557,7 +6557,7 @@
         <v>438</v>
       </c>
     </row>
-    <row r="100" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A100">
         <v>46</v>
       </c>
@@ -6598,7 +6598,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="101" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A101">
         <v>45</v>
       </c>
@@ -6642,7 +6642,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="102" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A102">
         <v>44</v>
       </c>
@@ -6683,7 +6683,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="103" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A103">
         <v>43</v>
       </c>
@@ -6733,7 +6733,7 @@
         <v>550</v>
       </c>
     </row>
-    <row r="104" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A104">
         <v>42</v>
       </c>
@@ -6774,7 +6774,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="105" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A105">
         <v>41</v>
       </c>
@@ -6815,7 +6815,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="106" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A106">
         <v>40</v>
       </c>
@@ -6859,7 +6859,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="107" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A107">
         <v>39</v>
       </c>
@@ -6903,7 +6903,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="108" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A108">
         <v>38</v>
       </c>
@@ -6947,7 +6947,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="109" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A109">
         <v>37</v>
       </c>
@@ -6991,7 +6991,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="110" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A110">
         <v>36</v>
       </c>
@@ -7032,7 +7032,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="111" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A111">
         <v>35</v>
       </c>
@@ -7076,7 +7076,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="112" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A112">
         <v>34</v>
       </c>
@@ -7117,7 +7117,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="113" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A113">
         <v>33</v>
       </c>
@@ -7158,7 +7158,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="114" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A114">
         <v>32</v>
       </c>
@@ -7205,7 +7205,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="115" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A115">
         <v>31</v>
       </c>
@@ -7246,7 +7246,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="116" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A116">
         <v>30</v>
       </c>
@@ -7287,7 +7287,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="117" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A117">
         <v>29</v>
       </c>
@@ -7331,7 +7331,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="118" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A118">
         <v>28</v>
       </c>
@@ -7375,7 +7375,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="119" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A119">
         <v>27</v>
       </c>
@@ -7422,7 +7422,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="120" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A120">
         <v>26</v>
       </c>
@@ -7463,7 +7463,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="121" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A121">
         <v>25</v>
       </c>
@@ -7504,7 +7504,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="122" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A122">
         <v>24</v>
       </c>
@@ -7545,7 +7545,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="123" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A123">
         <v>23</v>
       </c>
@@ -7586,7 +7586,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="124" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A124">
         <v>22</v>
       </c>
@@ -7627,7 +7627,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="125" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A125">
         <v>21</v>
       </c>
@@ -7668,7 +7668,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="126" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A126">
         <v>20</v>
       </c>
@@ -7709,7 +7709,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="127" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A127">
         <v>19</v>
       </c>
@@ -7750,7 +7750,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="128" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A128">
         <v>18</v>
       </c>
@@ -7791,7 +7791,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="129" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A129">
         <v>17</v>
       </c>
@@ -7832,7 +7832,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="130" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A130">
         <v>16</v>
       </c>
@@ -7873,7 +7873,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="131" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A131">
         <v>15</v>
       </c>
@@ -7917,7 +7917,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="132" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A132">
         <v>14</v>
       </c>
@@ -7961,7 +7961,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="133" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A133">
         <v>13</v>
       </c>
@@ -8002,7 +8002,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="134" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A134">
         <v>12</v>
       </c>
@@ -8043,7 +8043,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="135" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A135">
         <v>11</v>
       </c>
@@ -8084,7 +8084,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="136" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A136">
         <v>10</v>
       </c>
@@ -8128,7 +8128,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="137" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A137">
         <v>9</v>
       </c>
@@ -8169,7 +8169,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="138" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A138">
         <v>8</v>
       </c>
@@ -8210,7 +8210,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="139" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A139">
         <v>7</v>
       </c>
@@ -8254,7 +8254,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="140" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A140">
         <v>6</v>
       </c>
@@ -8298,7 +8298,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="141" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A141">
         <v>5</v>
       </c>
@@ -8339,7 +8339,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="142" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A142">
         <v>4</v>
       </c>
@@ -8386,7 +8386,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="143" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A143">
         <v>3</v>
       </c>
@@ -8427,7 +8427,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="144" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A144">
         <v>2</v>
       </c>
@@ -8471,7 +8471,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="145" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A145">
         <v>1</v>
       </c>
@@ -8515,7 +8515,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="146" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:15" x14ac:dyDescent="0.35">
       <c r="O146">
         <f>SUM(O2:O145)</f>
         <v>22</v>
@@ -8534,9 +8534,9 @@
       <selection activeCell="O2" sqref="O2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>227</v>
       </c>
@@ -8559,7 +8559,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>16</v>
       </c>
@@ -8591,7 +8591,7 @@
         <v>541</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>25</v>
       </c>
@@ -8599,22 +8599,22 @@
         <v>376</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>107</v>
       </c>
@@ -8622,22 +8622,22 @@
         <v>108</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>307</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>289</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>290</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>387</v>
       </c>

</xml_diff>

<commit_message>
graphic categories over time
</commit_message>
<xml_diff>
--- a/data/raw/collected_metadata/metadata_avis.xlsx
+++ b/data/raw/collected_metadata/metadata_avis.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://genes-my.sharepoint.com/personal/lmaurice_ensae_fr/Documents/CCNE/Analyse/CCNE/data/raw/collected_metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1572" documentId="11_AD4D9D64A577C15A4A54185C681B52125BDEDD8A" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{27808F61-6838-4BF8-8FA7-EF410B0ACC4D}"/>
+  <xr:revisionPtr revIDLastSave="1581" documentId="11_AD4D9D64A577C15A4A54185C681B52125BDEDD8A" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F7029276-02ED-42FE-9F9D-8B8636E92832}"/>
   <bookViews>
     <workbookView xWindow="19090" yWindow="-940" windowWidth="22620" windowHeight="13500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2023,22 +2023,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P146"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView tabSelected="1" topLeftCell="A124" zoomScale="75" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J140" sqref="J140"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="14.42578125" customWidth="1"/>
-    <col min="3" max="3" width="20.140625" customWidth="1"/>
-    <col min="4" max="4" width="62.5703125" customWidth="1"/>
-    <col min="5" max="5" width="43" customWidth="1"/>
-    <col min="6" max="6" width="16.7109375" customWidth="1"/>
-    <col min="7" max="7" width="7.5703125" customWidth="1"/>
-    <col min="8" max="8" width="9" customWidth="1"/>
-    <col min="9" max="9" width="11.85546875" customWidth="1"/>
-    <col min="10" max="10" width="30.42578125" customWidth="1"/>
+    <col min="2" max="2" width="0.42578125" customWidth="1"/>
+    <col min="3" max="3" width="20.140625" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="62.5703125" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="0.28515625" customWidth="1"/>
+    <col min="6" max="6" width="16.7109375" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="7.5703125" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="9" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="40.42578125" customWidth="1"/>
+    <col min="10" max="10" width="102.28515625" customWidth="1"/>
     <col min="11" max="11" width="17.28515625" customWidth="1"/>
+    <col min="12" max="12" width="1.5703125" customWidth="1"/>
+    <col min="13" max="13" width="38" customWidth="1"/>
+    <col min="14" max="14" width="1.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
completion citation up to avis 104
</commit_message>
<xml_diff>
--- a/data/raw/collected_metadata/metadata_avis.xlsx
+++ b/data/raw/collected_metadata/metadata_avis.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://genes-my.sharepoint.com/personal/lmaurice_ensae_fr/Documents/CCNE/Analyse/CCNE/data/raw/collected_metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1681" documentId="11_AD4D9D64A577C15A4A54185C681B52125BDEDD8A" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{96C35D3C-F105-4929-8BFA-864BCC852876}"/>
+  <xr:revisionPtr revIDLastSave="1691" documentId="11_AD4D9D64A577C15A4A54185C681B52125BDEDD8A" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{42E1AB43-8EF3-4FC8-844E-D136906DCBE6}"/>
   <bookViews>
-    <workbookView xWindow="18885" yWindow="0" windowWidth="10020" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="metadata" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1067" uniqueCount="559">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1070" uniqueCount="562">
   <si>
     <t>num</t>
   </si>
@@ -1716,6 +1716,15 @@
   </si>
   <si>
     <t>84;27;77</t>
+  </si>
+  <si>
+    <t>94;95;47</t>
+  </si>
+  <si>
+    <t>97;44</t>
+  </si>
+  <si>
+    <t>87;98;91;101</t>
   </si>
 </sst>
 </file>
@@ -2042,8 +2051,8 @@
   <dimension ref="A1:Q146"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A28" zoomScale="75" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="Q1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="Q52" sqref="Q52"/>
+      <pane xSplit="1" topLeftCell="P1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="Q43" sqref="Q43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3504,7 +3513,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>113</v>
       </c>
@@ -3545,7 +3554,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>112</v>
       </c>
@@ -3589,7 +3598,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>111</v>
       </c>
@@ -3636,7 +3645,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>110</v>
       </c>
@@ -3680,7 +3689,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>109</v>
       </c>
@@ -3724,7 +3733,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>108</v>
       </c>
@@ -3771,7 +3780,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>107</v>
       </c>
@@ -3812,7 +3821,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>106</v>
       </c>
@@ -3859,7 +3868,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>105</v>
       </c>
@@ -3903,7 +3912,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>104</v>
       </c>
@@ -3949,8 +3958,11 @@
       <c r="P42" t="s">
         <v>204</v>
       </c>
-    </row>
-    <row r="43" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q42" t="s">
+        <v>561</v>
+      </c>
+    </row>
+    <row r="43" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>103</v>
       </c>
@@ -3999,8 +4011,11 @@
       <c r="P43" t="s">
         <v>197</v>
       </c>
-    </row>
-    <row r="44" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q43" t="s">
+        <v>560</v>
+      </c>
+    </row>
+    <row r="44" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>102</v>
       </c>
@@ -4049,8 +4064,11 @@
       <c r="P44" t="s">
         <v>202</v>
       </c>
-    </row>
-    <row r="45" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q44" t="s">
+        <v>559</v>
+      </c>
+    </row>
+    <row r="45" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>101</v>
       </c>
@@ -4090,8 +4108,11 @@
       <c r="O45">
         <v>0</v>
       </c>
-    </row>
-    <row r="46" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q45">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="46" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>100</v>
       </c>
@@ -4141,7 +4162,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="47" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>99</v>
       </c>
@@ -4188,7 +4209,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="48" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>98</v>
       </c>
@@ -4230,6 +4251,9 @@
       </c>
       <c r="O48">
         <v>0</v>
+      </c>
+      <c r="Q48">
+        <v>77</v>
       </c>
     </row>
     <row r="49" spans="1:17" x14ac:dyDescent="0.25">
@@ -4280,6 +4304,9 @@
       </c>
       <c r="P49" t="s">
         <v>239</v>
+      </c>
+      <c r="Q49">
+        <v>83</v>
       </c>
     </row>
     <row r="50" spans="1:17" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
une fichier de recat des citations, graphiques macro, graphiques interactifs et app ready seul défaut : le degree in or out pour ccne
</commit_message>
<xml_diff>
--- a/data/raw/collected_metadata/metadata_avis.xlsx
+++ b/data/raw/collected_metadata/metadata_avis.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://genes-my.sharepoint.com/personal/lmaurice_ensae_fr/Documents/CCNE/Analyse/CCNE/data/raw/collected_metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1769" documentId="11_AD4D9D64A577C15A4A54185C681B52125BDEDD8A" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1EC7A60C-312F-494B-95A8-9551C165CF03}"/>
+  <xr:revisionPtr revIDLastSave="1833" documentId="11_AD4D9D64A577C15A4A54185C681B52125BDEDD8A" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B438FDF7-8893-48B8-BF19-BB56C99E235F}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1103" uniqueCount="595">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1126" uniqueCount="618">
   <si>
     <t>num</t>
   </si>
@@ -1824,6 +1824,75 @@
   </si>
   <si>
     <t>3;8;18;19;20;24</t>
+  </si>
+  <si>
+    <t>4;5;17;25;30</t>
+  </si>
+  <si>
+    <t>39;40</t>
+  </si>
+  <si>
+    <t>1;23</t>
+  </si>
+  <si>
+    <t>8;9;16;21</t>
+  </si>
+  <si>
+    <t>46;42;24</t>
+  </si>
+  <si>
+    <t>34;39;43;38</t>
+  </si>
+  <si>
+    <t>57;58</t>
+  </si>
+  <si>
+    <t>1;52;53;54;19;8;56;46;4;9;25;38;35;36;41;39;40;43;44;45;49;50;51;54</t>
+  </si>
+  <si>
+    <t>26;42;58;57;59</t>
+  </si>
+  <si>
+    <t>24;42;60</t>
+  </si>
+  <si>
+    <t>60;54;53</t>
+  </si>
+  <si>
+    <t>5;25;37;46;19;42;65;57</t>
+  </si>
+  <si>
+    <t>58;46</t>
+  </si>
+  <si>
+    <t>58;70</t>
+  </si>
+  <si>
+    <t>8;19;60;70</t>
+  </si>
+  <si>
+    <t>72;42</t>
+  </si>
+  <si>
+    <t>25;70;72</t>
+  </si>
+  <si>
+    <t>41;57;17</t>
+  </si>
+  <si>
+    <t>58;73;55;70;71;2;12;57;38</t>
+  </si>
+  <si>
+    <t>45;35;75</t>
+  </si>
+  <si>
+    <t>76;46</t>
+  </si>
+  <si>
+    <t>86;63;65;70;84</t>
+  </si>
+  <si>
+    <t>112;116;109;77;127;105;46;124;120;115;122;126;90;113;26;63;87;108;121;128</t>
   </si>
 </sst>
 </file>
@@ -2149,16 +2218,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q145"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" zoomScale="75" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="75" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="A64" sqref="A64:XFD64"/>
+      <selection pane="topRight" activeCell="Q17" sqref="Q17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="5.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22" hidden="1" customWidth="1"/>
+    <col min="3" max="3" width="9.5703125" customWidth="1"/>
     <col min="4" max="4" width="46.85546875" customWidth="1"/>
     <col min="5" max="5" width="8.5703125" customWidth="1"/>
     <col min="6" max="6" width="1" customWidth="1"/>
@@ -2996,6 +3065,9 @@
       <c r="O17">
         <v>0</v>
       </c>
+      <c r="Q17" t="s">
+        <v>617</v>
+      </c>
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A18">
@@ -4368,6 +4440,9 @@
       <c r="P46" t="s">
         <v>222</v>
       </c>
+      <c r="Q46">
+        <v>90</v>
+      </c>
     </row>
     <row r="47" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A47">
@@ -4954,7 +5029,7 @@
         <v>165</v>
       </c>
       <c r="N58" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O58">
         <v>0</v>
@@ -5003,6 +5078,9 @@
       <c r="O59">
         <v>0</v>
       </c>
+      <c r="Q59" t="s">
+        <v>616</v>
+      </c>
     </row>
     <row r="60" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A60">
@@ -5100,6 +5178,9 @@
       <c r="O61">
         <v>0</v>
       </c>
+      <c r="Q61">
+        <v>79</v>
+      </c>
     </row>
     <row r="62" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A62">
@@ -5203,6 +5284,9 @@
       <c r="P63" t="s">
         <v>300</v>
       </c>
+      <c r="Q63" t="s">
+        <v>615</v>
+      </c>
     </row>
     <row r="64" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A64">
@@ -5257,7 +5341,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="65" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>81</v>
       </c>
@@ -5303,8 +5387,11 @@
       <c r="O65">
         <v>0</v>
       </c>
-    </row>
-    <row r="66" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q65" t="s">
+        <v>614</v>
+      </c>
+    </row>
+    <row r="66" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>80</v>
       </c>
@@ -5353,8 +5440,11 @@
       <c r="P66" t="s">
         <v>313</v>
       </c>
-    </row>
-    <row r="67" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q66">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="67" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>79</v>
       </c>
@@ -5400,8 +5490,11 @@
       <c r="O67">
         <v>0</v>
       </c>
-    </row>
-    <row r="68" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q67" t="s">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="68" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>78</v>
       </c>
@@ -5450,8 +5543,11 @@
       <c r="P68" t="s">
         <v>321</v>
       </c>
-    </row>
-    <row r="69" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q68" t="s">
+        <v>612</v>
+      </c>
+    </row>
+    <row r="69" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>77</v>
       </c>
@@ -5495,7 +5591,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="70" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>76</v>
       </c>
@@ -5541,8 +5637,11 @@
       <c r="O70">
         <v>0</v>
       </c>
-    </row>
-    <row r="71" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q70" t="s">
+        <v>611</v>
+      </c>
+    </row>
+    <row r="71" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>75</v>
       </c>
@@ -5588,8 +5687,11 @@
       <c r="P71" t="s">
         <v>330</v>
       </c>
-    </row>
-    <row r="72" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q71" t="s">
+        <v>610</v>
+      </c>
+    </row>
+    <row r="72" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>74</v>
       </c>
@@ -5639,7 +5741,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="73" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>73</v>
       </c>
@@ -5688,8 +5790,11 @@
       <c r="P73" t="s">
         <v>335</v>
       </c>
-    </row>
-    <row r="74" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q73">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="74" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>72</v>
       </c>
@@ -5735,8 +5840,11 @@
       <c r="P74" t="s">
         <v>342</v>
       </c>
-    </row>
-    <row r="75" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q74" t="s">
+        <v>609</v>
+      </c>
+    </row>
+    <row r="75" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>71</v>
       </c>
@@ -5785,8 +5893,11 @@
       <c r="P75" t="s">
         <v>346</v>
       </c>
-    </row>
-    <row r="76" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q75" t="s">
+        <v>608</v>
+      </c>
+    </row>
+    <row r="76" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>70</v>
       </c>
@@ -5826,8 +5937,11 @@
       <c r="O76">
         <v>0</v>
       </c>
-    </row>
-    <row r="77" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q76" t="s">
+        <v>607</v>
+      </c>
+    </row>
+    <row r="77" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>69</v>
       </c>
@@ -5867,8 +5981,11 @@
       <c r="O77">
         <v>0</v>
       </c>
-    </row>
-    <row r="78" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q77">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="78" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>68</v>
       </c>
@@ -5917,8 +6034,11 @@
       <c r="P78" t="s">
         <v>353</v>
       </c>
-    </row>
-    <row r="79" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q78" t="s">
+        <v>606</v>
+      </c>
+    </row>
+    <row r="79" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>67</v>
       </c>
@@ -5964,8 +6084,11 @@
       <c r="P79" t="s">
         <v>357</v>
       </c>
-    </row>
-    <row r="80" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q79" t="s">
+        <v>605</v>
+      </c>
+    </row>
+    <row r="80" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>66</v>
       </c>
@@ -6015,7 +6138,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="81" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>65</v>
       </c>
@@ -6061,8 +6184,11 @@
       <c r="P81" t="s">
         <v>363</v>
       </c>
-    </row>
-    <row r="82" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q81" t="s">
+        <v>604</v>
+      </c>
+    </row>
+    <row r="82" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>64</v>
       </c>
@@ -6103,7 +6229,7 @@
         <v>42</v>
       </c>
       <c r="N82" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O82">
         <v>0</v>
@@ -6112,7 +6238,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="83" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>63</v>
       </c>
@@ -6155,8 +6281,11 @@
       <c r="P83" t="s">
         <v>369</v>
       </c>
-    </row>
-    <row r="84" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q83" t="s">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="84" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>62</v>
       </c>
@@ -6205,8 +6334,11 @@
       <c r="P84" t="s">
         <v>372</v>
       </c>
-    </row>
-    <row r="85" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q84">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="85" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>61</v>
       </c>
@@ -6247,7 +6379,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>60</v>
       </c>
@@ -6290,8 +6422,11 @@
       <c r="O86">
         <v>0</v>
       </c>
-    </row>
-    <row r="87" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q86" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="87" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>59</v>
       </c>
@@ -6331,8 +6466,11 @@
       <c r="O87">
         <v>5</v>
       </c>
-    </row>
-    <row r="88" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q87" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="88" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>58</v>
       </c>
@@ -6375,8 +6513,11 @@
       <c r="O88">
         <v>0</v>
       </c>
-    </row>
-    <row r="89" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q88" t="s">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="89" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>57</v>
       </c>
@@ -6416,8 +6557,11 @@
       <c r="O89">
         <v>4</v>
       </c>
-    </row>
-    <row r="90" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q89" t="s">
+        <v>599</v>
+      </c>
+    </row>
+    <row r="90" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>56</v>
       </c>
@@ -6458,7 +6602,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>55</v>
       </c>
@@ -6502,7 +6646,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>54</v>
       </c>
@@ -6545,8 +6689,11 @@
       <c r="O92">
         <v>0</v>
       </c>
-    </row>
-    <row r="93" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q92" t="s">
+        <v>598</v>
+      </c>
+    </row>
+    <row r="93" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>53</v>
       </c>
@@ -6586,8 +6733,11 @@
       <c r="O93">
         <v>0</v>
       </c>
-    </row>
-    <row r="94" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q93" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="94" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>52</v>
       </c>
@@ -6627,8 +6777,11 @@
       <c r="O94">
         <v>0</v>
       </c>
-    </row>
-    <row r="95" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q94">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="95" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>51</v>
       </c>
@@ -6671,8 +6824,11 @@
       <c r="P95" t="s">
         <v>395</v>
       </c>
-    </row>
-    <row r="96" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q95" t="s">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="96" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>50</v>
       </c>
@@ -6714,6 +6870,9 @@
       </c>
       <c r="O96">
         <v>0</v>
+      </c>
+      <c r="Q96">
+        <v>49</v>
       </c>
     </row>
     <row r="97" spans="1:17" x14ac:dyDescent="0.25">
@@ -6897,6 +7056,9 @@
       <c r="O100">
         <v>0</v>
       </c>
+      <c r="Q100" t="s">
+        <v>595</v>
+      </c>
     </row>
     <row r="101" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A101">
@@ -6940,6 +7102,9 @@
       </c>
       <c r="O101">
         <v>0</v>
+      </c>
+      <c r="Q101">
+        <v>39</v>
       </c>
     </row>
     <row r="102" spans="1:17" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
llm: gpt for 6 classes
</commit_message>
<xml_diff>
--- a/data/raw/collected_metadata/metadata_avis.xlsx
+++ b/data/raw/collected_metadata/metadata_avis.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://genes-my.sharepoint.com/personal/lmaurice_ensae_fr/Documents/CCNE/Analyse/CCNE/data/raw/collected_metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1833" documentId="11_AD4D9D64A577C15A4A54185C681B52125BDEDD8A" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B438FDF7-8893-48B8-BF19-BB56C99E235F}"/>
+  <xr:revisionPtr revIDLastSave="1835" documentId="11_AD4D9D64A577C15A4A54185C681B52125BDEDD8A" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F83D5DE3-1E80-4810-BBC8-9457DB148488}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="15" yWindow="15" windowWidth="28770" windowHeight="15450" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="metadata" sheetId="1" r:id="rId1"/>
@@ -2218,9 +2218,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q145"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="75" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="Q17" sqref="Q17"/>
+      <selection pane="topRight" activeCell="J1" activeCellId="1" sqref="A1:A1048576 J1:J1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>